<commit_message>
boton leave para mercancia
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla11\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2726BA-E56F-429D-B492-3A7667B2C978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFA4943-1C00-48BE-B184-85DE7F69486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>MSIDN</t>
   </si>
@@ -238,9 +238,6 @@
     <t>3046010569</t>
   </si>
   <si>
-    <t>3046008593</t>
-  </si>
-  <si>
     <t>732111193280551</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
   </si>
   <si>
     <t>732111193278863</t>
-  </si>
-  <si>
-    <t>3045987650</t>
   </si>
   <si>
     <t>732111193278858</t>
@@ -756,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -802,19 +796,19 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>24</v>
@@ -826,7 +820,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1">
@@ -850,7 +844,7 @@
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>59</v>
@@ -875,10 +869,10 @@
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -887,7 +881,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>57</v>
@@ -900,10 +894,10 @@
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -919,7 +913,7 @@
     </row>
     <row r="7" spans="1:9" s="11" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -970,25 +964,25 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>48</v>
@@ -999,16 +993,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>52</v>
@@ -1017,7 +1011,7 @@
         <v>43</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>49</v>
@@ -1028,13 +1022,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
@@ -1042,13 +1036,13 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1">
@@ -1056,13 +1050,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1070,13 +1064,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realizan ajuste en tiempos
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla11\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla11\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2726BA-E56F-429D-B492-3A7667B2C978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D486B1-C12A-408B-9FCA-2A1D300632ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 11" sheetId="2" r:id="rId1"/>
@@ -286,9 +286,6 @@
     <t>562160567</t>
   </si>
   <si>
-    <t>410868055</t>
-  </si>
-  <si>
     <t>382742205</t>
   </si>
   <si>
@@ -307,18 +304,6 @@
     <t>http://10.65.45.14:7001/gatewaycbs/BcServicesInt?WSDL</t>
   </si>
   <si>
-    <t>3045975044</t>
-  </si>
-  <si>
-    <t>732111193278871</t>
-  </si>
-  <si>
-    <t>3045987678</t>
-  </si>
-  <si>
-    <t>732111193278863</t>
-  </si>
-  <si>
     <t>3045987650</t>
   </si>
   <si>
@@ -326,6 +311,21 @@
   </si>
   <si>
     <t>3045984556</t>
+  </si>
+  <si>
+    <t>3046010523</t>
+  </si>
+  <si>
+    <t>732111193280544</t>
+  </si>
+  <si>
+    <t>3052749177</t>
+  </si>
+  <si>
+    <t>732111324709512</t>
+  </si>
+  <si>
+    <t>484303795</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -439,6 +439,8 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -754,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -811,10 +813,10 @@
         <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>24</v>
@@ -903,7 +905,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -973,10 +975,10 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>53</v>
@@ -999,16 +1001,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>52</v>
@@ -1028,13 +1030,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
@@ -1042,7 +1044,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>97</v>
@@ -1056,13 +1058,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1072,12 +1074,15 @@
       <c r="B14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>70</v>
+      <c r="C14" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>72</v>
       </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Se agregan nuevos casos de uso, 1. Cesion de contrato nit a nit con cambio a plan pospago empresarial 5.3 y 2. activacion nintendo con cliente nit
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla11\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFA4943-1C00-48BE-B184-85DE7F69486F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EEAC9E-E56A-4F21-88A2-AA27131749DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>MSIDN</t>
   </si>
@@ -235,91 +235,97 @@
     <t xml:space="preserve">732111324707277 </t>
   </si>
   <si>
+    <t>69883703</t>
+  </si>
+  <si>
+    <t>345769284</t>
+  </si>
+  <si>
+    <t>732111193278721</t>
+  </si>
+  <si>
+    <t>http://10.65.50.11:8280/portal/CRMPortal/Venta</t>
+  </si>
+  <si>
+    <t>http://10.65.50.9:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>http://10.65.50.9:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.65.39.16</t>
+  </si>
+  <si>
+    <t>10.65.39.15</t>
+  </si>
+  <si>
+    <t>10.69.34.11</t>
+  </si>
+  <si>
+    <t>DESEPOS</t>
+  </si>
+  <si>
+    <t>10.65.50.8</t>
+  </si>
+  <si>
+    <t>562160567</t>
+  </si>
+  <si>
+    <t>410868055</t>
+  </si>
+  <si>
+    <t>382742205</t>
+  </si>
+  <si>
+    <t>10630392</t>
+  </si>
+  <si>
+    <t>876431876</t>
+  </si>
+  <si>
+    <t>DEV10G</t>
+  </si>
+  <si>
+    <t>http://10.65.45.14:7001/gatewaymgint/GatewayMGWSInt</t>
+  </si>
+  <si>
+    <t>http://10.65.45.14:7001/gatewaycbs/BcServicesInt?WSDL</t>
+  </si>
+  <si>
+    <t>3045987650</t>
+  </si>
+  <si>
     <t>3046010569</t>
   </si>
   <si>
+    <t>3046010523</t>
+  </si>
+  <si>
+    <t>732111193278858</t>
+  </si>
+  <si>
     <t>732111193280551</t>
   </si>
   <si>
-    <t>732111193280535</t>
-  </si>
-  <si>
-    <t>69883703</t>
-  </si>
-  <si>
-    <t>345769284</t>
-  </si>
-  <si>
-    <t>732111193278721</t>
-  </si>
-  <si>
-    <t>http://10.65.50.11:8280/portal/CRMPortal/Venta</t>
-  </si>
-  <si>
-    <t>http://10.65.50.9:8180/tigo-pos-web/index.jsp</t>
-  </si>
-  <si>
-    <t>http://10.65.50.9:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>http://10.65.50.9:8180/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
-  </si>
-  <si>
-    <t>10.65.39.16</t>
-  </si>
-  <si>
-    <t>10.65.39.15</t>
-  </si>
-  <si>
-    <t>10.69.34.11</t>
-  </si>
-  <si>
-    <t>DESEPOS</t>
-  </si>
-  <si>
-    <t>10.65.50.8</t>
-  </si>
-  <si>
-    <t>562160567</t>
-  </si>
-  <si>
-    <t>410868055</t>
-  </si>
-  <si>
-    <t>382742205</t>
-  </si>
-  <si>
-    <t>10630392</t>
-  </si>
-  <si>
-    <t>876431876</t>
-  </si>
-  <si>
-    <t>DEV10G</t>
-  </si>
-  <si>
-    <t>http://10.65.45.14:7001/gatewaymgint/GatewayMGWSInt</t>
-  </si>
-  <si>
-    <t>http://10.65.45.14:7001/gatewaycbs/BcServicesInt?WSDL</t>
-  </si>
-  <si>
-    <t>3045975044</t>
-  </si>
-  <si>
-    <t>732111193278871</t>
-  </si>
-  <si>
-    <t>3045987678</t>
-  </si>
-  <si>
-    <t>732111193278863</t>
-  </si>
-  <si>
-    <t>732111193278858</t>
-  </si>
-  <si>
-    <t>3045984556</t>
+    <t>732111193280544</t>
+  </si>
+  <si>
+    <t>3046008593</t>
+  </si>
+  <si>
+    <t>http://10.65.50.8:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl?wsdl</t>
+  </si>
+  <si>
+    <t>732111324709675</t>
+  </si>
+  <si>
+    <t>3052754293</t>
+  </si>
+  <si>
+    <t>3052754289</t>
+  </si>
+  <si>
+    <t>732111324709674</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -433,6 +439,8 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -750,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -796,19 +804,19 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>24</v>
@@ -820,7 +828,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1">
@@ -844,7 +852,7 @@
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>59</v>
@@ -869,10 +877,10 @@
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -881,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>57</v>
@@ -894,10 +902,10 @@
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -913,7 +921,7 @@
     </row>
     <row r="7" spans="1:9" s="11" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -964,25 +972,25 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>48</v>
@@ -993,16 +1001,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>52</v>
@@ -1011,7 +1019,7 @@
         <v>43</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>49</v>
@@ -1022,13 +1030,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
@@ -1036,13 +1044,13 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1">
@@ -1050,13 +1058,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1064,13 +1072,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega nueva mercancia e inventario
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla11\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EEAC9E-E56A-4F21-88A2-AA27131749DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118D36B3-8F04-4987-A553-B55A47057437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
   <si>
     <t>MSIDN</t>
   </si>
@@ -298,18 +298,9 @@
     <t>3046010569</t>
   </si>
   <si>
-    <t>3046010523</t>
-  </si>
-  <si>
-    <t>732111193278858</t>
-  </si>
-  <si>
     <t>732111193280551</t>
   </si>
   <si>
-    <t>732111193280544</t>
-  </si>
-  <si>
     <t>3046008593</t>
   </si>
   <si>
@@ -319,13 +310,46 @@
     <t>732111324709675</t>
   </si>
   <si>
-    <t>3052754293</t>
-  </si>
-  <si>
     <t>3052754289</t>
   </si>
   <si>
     <t>732111324709674</t>
+  </si>
+  <si>
+    <t>3052749177</t>
+  </si>
+  <si>
+    <t>3052754285</t>
+  </si>
+  <si>
+    <t>732111324709512</t>
+  </si>
+  <si>
+    <t>732111324709673</t>
+  </si>
+  <si>
+    <t>3045984556</t>
+  </si>
+  <si>
+    <t>3046008586</t>
+  </si>
+  <si>
+    <t>732111324709676</t>
+  </si>
+  <si>
+    <t>732111193278871</t>
+  </si>
+  <si>
+    <t>client nit a nit</t>
+  </si>
+  <si>
+    <t>988154393</t>
+  </si>
+  <si>
+    <t>36844580</t>
+  </si>
+  <si>
+    <t>914355426</t>
   </si>
 </sst>
 </file>
@@ -414,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -440,7 +464,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -756,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -828,7 +851,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1">
@@ -975,10 +998,10 @@
         <v>80</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>36</v>
@@ -1004,13 +1027,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>52</v>
@@ -1033,10 +1056,10 @@
         <v>82</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
@@ -1050,7 +1073,10 @@
         <v>88</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1">
@@ -1064,7 +1090,10 @@
         <v>89</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1074,11 +1103,39 @@
       <c r="B14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega la clase PagoEquiposActions y PagoEquiposPage y se implementan los metodos para legalizar las lineas activas
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla11\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla11 - copia\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D486B1-C12A-408B-9FCA-2A1D300632ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B451E7-5587-4D77-A5D5-EE66789A39A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 11" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
   <si>
     <t>MSIDN</t>
   </si>
@@ -238,9 +238,6 @@
     <t>3046010569</t>
   </si>
   <si>
-    <t>3046008593</t>
-  </si>
-  <si>
     <t>732111193280551</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>http://10.65.50.9:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
-    <t>http://10.65.50.9:8180/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
-  </si>
-  <si>
     <t>10.65.39.16</t>
   </si>
   <si>
@@ -283,18 +277,9 @@
     <t>10.65.50.8</t>
   </si>
   <si>
-    <t>562160567</t>
-  </si>
-  <si>
     <t>382742205</t>
   </si>
   <si>
-    <t>10630392</t>
-  </si>
-  <si>
-    <t>876431876</t>
-  </si>
-  <si>
     <t>DEV10G</t>
   </si>
   <si>
@@ -304,28 +289,49 @@
     <t>http://10.65.45.14:7001/gatewaycbs/BcServicesInt?WSDL</t>
   </si>
   <si>
-    <t>3045987650</t>
-  </si>
-  <si>
-    <t>732111193278858</t>
-  </si>
-  <si>
-    <t>3045984556</t>
-  </si>
-  <si>
     <t>3046010523</t>
   </si>
   <si>
     <t>732111193280544</t>
   </si>
   <si>
+    <t>http://10.65.50.8:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl?wsdl</t>
+  </si>
+  <si>
+    <t>3046008587</t>
+  </si>
+  <si>
+    <t>3046008588</t>
+  </si>
+  <si>
+    <t>3046008589</t>
+  </si>
+  <si>
+    <t>970271477</t>
+  </si>
+  <si>
+    <t>285174897</t>
+  </si>
+  <si>
+    <t>1019093413</t>
+  </si>
+  <si>
+    <t>74885324</t>
+  </si>
+  <si>
+    <t>412036519</t>
+  </si>
+  <si>
+    <t>732111193278871</t>
+  </si>
+  <si>
+    <t>3046008586</t>
+  </si>
+  <si>
     <t>3052749177</t>
   </si>
   <si>
     <t>732111324709512</t>
-  </si>
-  <si>
-    <t>484303795</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -756,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -804,19 +810,19 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1">
       <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>24</v>
@@ -827,8 +833,8 @@
       <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>79</v>
+      <c r="I2" s="13" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1">
@@ -852,7 +858,7 @@
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>59</v>
@@ -877,10 +883,10 @@
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1">
       <c r="A5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -889,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>57</v>
@@ -902,10 +908,10 @@
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -921,7 +927,7 @@
     </row>
     <row r="7" spans="1:9" s="11" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -972,25 +978,25 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>48</v>
@@ -1001,16 +1007,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>52</v>
@@ -1019,7 +1025,7 @@
         <v>43</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>49</v>
@@ -1030,13 +1036,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
@@ -1044,13 +1050,13 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1">
@@ -1058,13 +1064,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1072,17 +1078,14 @@
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="13"/>
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1090,8 +1093,8 @@
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I2" r:id="rId5" xr:uid="{F95E11DB-0174-40E5-880B-10A9CAE9721D}"/>
-    <hyperlink ref="E2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId6" tooltip="http://10.65.50.8:8080/portabilidadserviceear-hpnpcommunicationsdelegateejb/npcrmwsimpl?wsdl" xr:uid="{26F08B90-7FDF-4300-AA54-9E9BC0236203}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>